<commit_message>
Updates cheatsheet to reflect trky v2.1
</commit_message>
<xml_diff>
--- a/corne/turkey/turkey_crkbd_cheatsheet.xlsx
+++ b/corne/turkey/turkey_crkbd_cheatsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\code\deltakeys\corne\turkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D89A393-96DC-4B85-9AD5-662BBE62DB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EFC356-1668-4327-95A4-A06203570233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17955" yWindow="5610" windowWidth="32160" windowHeight="21435" xr2:uid="{1E181743-8F83-467F-80E8-6554C7BEF26B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>Q</t>
   </si>
@@ -294,6 +294,51 @@
   </si>
   <si>
     <t>;: (GUI)</t>
+  </si>
+  <si>
+    <t>M PLAY</t>
+  </si>
+  <si>
+    <t>CUT</t>
+  </si>
+  <si>
+    <t>COPY</t>
+  </si>
+  <si>
+    <t>UNDO</t>
+  </si>
+  <si>
+    <t>PASTE</t>
+  </si>
+  <si>
+    <t>B BACK</t>
+  </si>
+  <si>
+    <t>B FRWD</t>
+  </si>
+  <si>
+    <t>M WH UP</t>
+  </si>
+  <si>
+    <t>M LEFT</t>
+  </si>
+  <si>
+    <t>M DOWN</t>
+  </si>
+  <si>
+    <t>M RIGHT</t>
+  </si>
+  <si>
+    <t>M WH DN</t>
+  </si>
+  <si>
+    <t>MB 1</t>
+  </si>
+  <si>
+    <t>MB 2</t>
+  </si>
+  <si>
+    <t>MB 3</t>
   </si>
 </sst>
 </file>
@@ -466,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,73 +525,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -555,16 +570,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -919,7 +925,7 @@
   <dimension ref="B1:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,201 +968,213 @@
         <v>68</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="L2" s="5"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
       <c r="S2" s="6"/>
       <c r="T2" s="5"/>
       <c r="U2" s="6"/>
-      <c r="V2" s="5"/>
+      <c r="V2" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="W2" s="6"/>
-      <c r="X2" s="7"/>
+      <c r="X2" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="5"/>
+      <c r="Z2" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="AA2" s="6"/>
-      <c r="AB2" s="7"/>
+      <c r="AB2" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="AC2" s="6"/>
-      <c r="AD2" s="7"/>
+      <c r="AD2" s="5"/>
     </row>
     <row r="3" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10" t="s">
+      <c r="K3" s="8"/>
+      <c r="L3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="8" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="9"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="10"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="7"/>
     </row>
     <row r="4" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="9">
         <v>7</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13">
+      <c r="E4" s="10"/>
+      <c r="F4" s="9">
         <v>8</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11">
+      <c r="G4" s="10"/>
+      <c r="H4" s="9">
         <v>9</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13">
+      <c r="I4" s="10"/>
+      <c r="J4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="13"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="9"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="15" t="s">
+      <c r="M5" s="12"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="16"/>
-      <c r="V5" s="15" t="s">
+      <c r="U5" s="12"/>
+      <c r="V5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="16"/>
-      <c r="X5" s="17" t="s">
+      <c r="W5" s="12"/>
+      <c r="X5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="15" t="s">
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="17" t="s">
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="17"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="11"/>
     </row>
     <row r="6" spans="2:30" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
     </row>
     <row r="7" spans="2:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1167,7 +1185,7 @@
         <v>72</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G7" s="6"/>
@@ -1175,215 +1193,227 @@
         <v>75</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
+      <c r="L7" s="5"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="7"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="5"/>
       <c r="S7" s="6"/>
-      <c r="T7" s="5"/>
+      <c r="T7" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="U7" s="6"/>
-      <c r="V7" s="5"/>
+      <c r="V7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="W7" s="6"/>
-      <c r="X7" s="7"/>
+      <c r="X7" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="5"/>
+      <c r="Z7" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="AA7" s="6"/>
-      <c r="AB7" s="7"/>
+      <c r="AB7" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="7"/>
+      <c r="AD7" s="5"/>
     </row>
     <row r="8" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="8" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10" t="s">
+      <c r="K8" s="8"/>
+      <c r="L8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="8" t="s">
+      <c r="M8" s="8"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="9"/>
-      <c r="V8" s="8" t="s">
+      <c r="U8" s="8"/>
+      <c r="V8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="9"/>
-      <c r="X8" s="10" t="s">
+      <c r="W8" s="8"/>
+      <c r="X8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="8" t="s">
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="10" t="s">
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="10"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="7"/>
     </row>
     <row r="9" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9">
         <v>4</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13">
+      <c r="E9" s="10"/>
+      <c r="F9" s="9">
         <v>5</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11">
+      <c r="G9" s="10"/>
+      <c r="H9" s="9">
         <v>6</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="11" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="U9" s="12"/>
-      <c r="V9" s="27" t="s">
+      <c r="U9" s="10"/>
+      <c r="V9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="W9" s="12"/>
-      <c r="X9" s="27" t="s">
+      <c r="W9" s="10"/>
+      <c r="X9" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="27" t="s">
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="27" t="s">
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AC9" s="12"/>
-      <c r="AD9" s="13"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="9"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="15" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17" t="s">
+      <c r="I10" s="12"/>
+      <c r="J10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="17" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17" t="s">
+      <c r="M10" s="12"/>
+      <c r="N10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="17" t="s">
+      <c r="O10" s="12"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="S10" s="16"/>
-      <c r="T10" s="15" t="s">
+      <c r="S10" s="12"/>
+      <c r="T10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="U10" s="16"/>
-      <c r="V10" s="15" t="s">
+      <c r="U10" s="12"/>
+      <c r="V10" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="W10" s="16"/>
-      <c r="X10" s="17" t="s">
+      <c r="W10" s="12"/>
+      <c r="X10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="15" t="s">
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="34" t="s">
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="17"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="11"/>
     </row>
     <row r="11" spans="2:30" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
     </row>
     <row r="12" spans="2:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -1394,7 +1424,7 @@
         <v>71</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="6"/>
@@ -1402,343 +1432,357 @@
         <v>76</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
+      <c r="L12" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="7"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="5"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="5"/>
+      <c r="T12" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="U12" s="6"/>
-      <c r="V12" s="5"/>
+      <c r="V12" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="W12" s="6"/>
-      <c r="X12" s="7"/>
+      <c r="X12" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="Y12" s="6"/>
-      <c r="Z12" s="5"/>
+      <c r="Z12" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="AA12" s="6"/>
-      <c r="AB12" s="7"/>
+      <c r="AB12" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="AC12" s="6"/>
-      <c r="AD12" s="7"/>
+      <c r="AD12" s="5"/>
     </row>
     <row r="13" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10" t="s">
+      <c r="I13" s="8"/>
+      <c r="J13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="8" t="s">
+      <c r="K13" s="8"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="U13" s="9"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="10"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="7"/>
     </row>
     <row r="14" spans="2:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9">
         <v>1</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13">
+      <c r="E14" s="10"/>
+      <c r="F14" s="9">
         <v>2</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11">
+      <c r="G14" s="10"/>
+      <c r="H14" s="9">
         <v>3</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="22" t="s">
+      <c r="I14" s="10"/>
+      <c r="J14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="11" t="s">
+      <c r="K14" s="10"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="U14" s="12"/>
-      <c r="V14" s="26" t="s">
+      <c r="U14" s="10"/>
+      <c r="V14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="W14" s="12"/>
-      <c r="X14" s="13" t="s">
+      <c r="W14" s="10"/>
+      <c r="X14" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="13"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="9"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="12"/>
+      <c r="H15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17" t="s">
+      <c r="I15" s="12"/>
+      <c r="J15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="17" t="s">
+      <c r="K15" s="12"/>
+      <c r="L15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="17" t="s">
+      <c r="M15" s="12"/>
+      <c r="N15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O15" s="16"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="17" t="s">
+      <c r="O15" s="12"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S15" s="16"/>
-      <c r="T15" s="15" t="s">
+      <c r="S15" s="12"/>
+      <c r="T15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="U15" s="16"/>
-      <c r="V15" s="15" t="s">
+      <c r="U15" s="12"/>
+      <c r="V15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="W15" s="16"/>
-      <c r="X15" s="17" t="s">
+      <c r="W15" s="12"/>
+      <c r="X15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="15" t="s">
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="17" t="s">
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AC15" s="16"/>
-      <c r="AD15" s="17"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="11"/>
     </row>
     <row r="16" spans="2:30" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-      <c r="AD16" s="16"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="37" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="37" t="s">
+      <c r="M18" s="12"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="U18" s="16"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="35" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="22" t="s">
+      <c r="M19" s="12"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="S19" s="16"/>
-      <c r="T19" s="36" t="s">
+      <c r="S19" s="12"/>
+      <c r="T19" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="U19" s="16"/>
-      <c r="V19" s="22" t="s">
+      <c r="U19" s="12"/>
+      <c r="V19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="W19" s="16"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
+      <c r="K20" s="12"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="17" t="s">
+      <c r="O20" s="12"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="S20" s="16"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="17" t="s">
+      <c r="S20" s="12"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="W20" s="16"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
     </row>
     <row r="21" spans="2:30" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>